<commit_message>
Added more figures of the TOG paper.
</commit_message>
<xml_diff>
--- a/HandForests/results.xlsx
+++ b/HandForests/results.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TOG_height_train" sheetId="6" r:id="rId1"/>
+    <sheet name="TOG_num_trees_train" sheetId="5" r:id="rId2"/>
+    <sheet name="TOG_height_test" sheetId="7" r:id="rId3"/>
+    <sheet name="TOG_num_trees_test" sheetId="4" r:id="rId4"/>
+    <sheet name="OLD_DATA" sheetId="1" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="40">
   <si>
     <t xml:space="preserve">Using data set hand_depth_data_28Jul2012.zip.  From a videostream of 11734 images, every second image was labeled and saved as a processed image.  Then every 4 of those </t>
   </si>
@@ -118,6 +120,27 @@
   </si>
   <si>
     <t>6T</t>
+  </si>
+  <si>
+    <t>Training Set</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>False_Pos</t>
+  </si>
+  <si>
+    <t>Num_Trees</t>
+  </si>
+  <si>
+    <t>False_Neg</t>
+  </si>
+  <si>
+    <t>num_hand_pixels</t>
   </si>
 </sst>
 </file>
@@ -352,11 +375,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91888256"/>
-        <c:axId val="91890432"/>
+        <c:axId val="119736576"/>
+        <c:axId val="119738752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91888256"/>
+        <c:axId val="119736576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -389,7 +412,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -403,12 +425,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91890432"/>
+        <c:crossAx val="119738752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91890432"/>
+        <c:axId val="119738752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -440,14 +462,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91888256"/>
+        <c:crossAx val="119736576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -513,7 +534,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$136</c:f>
+              <c:f>OLD_DATA!$R$136</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -528,7 +549,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$137:$L$140</c:f>
+              <c:f>OLD_DATA!$L$137:$L$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -549,7 +570,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$137:$R$140</c:f>
+              <c:f>OLD_DATA!$R$137:$R$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -575,7 +596,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$136</c:f>
+              <c:f>OLD_DATA!$U$136</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -586,7 +607,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$137:$L$140</c:f>
+              <c:f>OLD_DATA!$L$137:$L$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -607,7 +628,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$U$137:$U$140</c:f>
+              <c:f>OLD_DATA!$U$137:$U$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -636,11 +657,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96636928"/>
-        <c:axId val="96638848"/>
+        <c:axId val="122699136"/>
+        <c:axId val="122713600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96636928"/>
+        <c:axId val="122699136"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -664,7 +685,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -678,12 +698,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96638848"/>
+        <c:crossAx val="122713600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96638848"/>
+        <c:axId val="122713600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -715,14 +735,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96636928"/>
+        <c:crossAx val="122699136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -788,7 +807,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$164</c:f>
+              <c:f>OLD_DATA!$N$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -803,7 +822,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$165:$L$168</c:f>
+              <c:f>OLD_DATA!$L$165:$L$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -824,7 +843,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$165:$N$168</c:f>
+              <c:f>OLD_DATA!$N$165:$N$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -847,7 +866,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$164</c:f>
+              <c:f>OLD_DATA!$Q$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -858,7 +877,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$165:$L$168</c:f>
+              <c:f>OLD_DATA!$L$165:$L$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -879,7 +898,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$165:$Q$168</c:f>
+              <c:f>OLD_DATA!$Q$165:$Q$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -905,11 +924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96537216"/>
-        <c:axId val="96543488"/>
+        <c:axId val="122734848"/>
+        <c:axId val="122745216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96537216"/>
+        <c:axId val="122734848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -941,7 +960,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -955,12 +973,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96543488"/>
+        <c:crossAx val="122745216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96543488"/>
+        <c:axId val="122745216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -992,14 +1010,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96537216"/>
+        <c:crossAx val="122734848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1065,7 +1082,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$164</c:f>
+              <c:f>OLD_DATA!$R$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1080,7 +1097,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$165:$L$168</c:f>
+              <c:f>OLD_DATA!$L$165:$L$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1101,7 +1118,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$165:$R$168</c:f>
+              <c:f>OLD_DATA!$R$165:$R$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1124,7 +1141,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$164</c:f>
+              <c:f>OLD_DATA!$U$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1135,7 +1152,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$165:$L$168</c:f>
+              <c:f>OLD_DATA!$L$165:$L$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1156,7 +1173,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$U$165:$U$168</c:f>
+              <c:f>OLD_DATA!$U$165:$U$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1182,11 +1199,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96581120"/>
-        <c:axId val="96583040"/>
+        <c:axId val="122782848"/>
+        <c:axId val="122784768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96581120"/>
+        <c:axId val="122782848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1210,7 +1227,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1224,12 +1240,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96583040"/>
+        <c:crossAx val="122784768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96583040"/>
+        <c:axId val="122784768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -1261,14 +1277,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96581120"/>
+        <c:crossAx val="122782848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1334,7 +1349,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$231</c:f>
+              <c:f>OLD_DATA!$P$231</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1349,7 +1364,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$232:$F$236</c:f>
+              <c:f>OLD_DATA!$F$232:$F$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1373,7 +1388,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$232:$P$236</c:f>
+              <c:f>OLD_DATA!$P$232:$P$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1402,7 +1417,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$231</c:f>
+              <c:f>OLD_DATA!$S$231</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1413,7 +1428,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$232:$F$236</c:f>
+              <c:f>OLD_DATA!$F$232:$F$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1437,7 +1452,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$232:$S$236</c:f>
+              <c:f>OLD_DATA!$S$232:$S$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1469,11 +1484,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96707328"/>
-        <c:axId val="96709248"/>
+        <c:axId val="123826560"/>
+        <c:axId val="123828480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96707328"/>
+        <c:axId val="123826560"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1503,7 +1518,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1517,12 +1531,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96709248"/>
+        <c:crossAx val="123828480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96709248"/>
+        <c:axId val="123828480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1554,14 +1568,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96707328"/>
+        <c:crossAx val="123826560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1627,7 +1640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$231</c:f>
+              <c:f>OLD_DATA!$T$231</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1642,7 +1655,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$232:$F$236</c:f>
+              <c:f>OLD_DATA!$F$232:$F$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1666,7 +1679,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$232:$T$236</c:f>
+              <c:f>OLD_DATA!$T$232:$T$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1695,7 +1708,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$W$231</c:f>
+              <c:f>OLD_DATA!$W$231</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1706,7 +1719,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$232:$F$236</c:f>
+              <c:f>OLD_DATA!$F$232:$F$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1730,7 +1743,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$W$232:$W$236</c:f>
+              <c:f>OLD_DATA!$W$232:$W$236</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1762,11 +1775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98119040"/>
-        <c:axId val="98121216"/>
+        <c:axId val="123939840"/>
+        <c:axId val="123946112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98119040"/>
+        <c:axId val="123939840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1791,7 +1804,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1805,12 +1817,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="98121216"/>
+        <c:crossAx val="123946112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98121216"/>
+        <c:axId val="123946112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1842,14 +1854,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98119040"/>
+        <c:crossAx val="123939840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1915,7 +1926,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$260</c:f>
+              <c:f>OLD_DATA!$P$260</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1930,7 +1941,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$261:$O$263</c:f>
+              <c:f>OLD_DATA!$O$261:$O$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1948,7 +1959,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$261:$P$263</c:f>
+              <c:f>OLD_DATA!$P$261:$P$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1971,7 +1982,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$260</c:f>
+              <c:f>OLD_DATA!$S$260</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1982,7 +1993,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$261:$O$263</c:f>
+              <c:f>OLD_DATA!$O$261:$O$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2000,7 +2011,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$261:$S$263</c:f>
+              <c:f>OLD_DATA!$S$261:$S$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2026,11 +2037,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98134272"/>
-        <c:axId val="99287424"/>
+        <c:axId val="123975552"/>
+        <c:axId val="123985920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98134272"/>
+        <c:axId val="123975552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,12 +2083,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99287424"/>
+        <c:crossAx val="123985920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99287424"/>
+        <c:axId val="123985920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -2116,7 +2127,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98134272"/>
+        <c:crossAx val="123975552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2182,7 +2193,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$260</c:f>
+              <c:f>OLD_DATA!$T$260</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2197,7 +2208,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$261:$O$263</c:f>
+              <c:f>OLD_DATA!$O$261:$O$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2215,7 +2226,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$261:$T$263</c:f>
+              <c:f>OLD_DATA!$T$261:$T$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2238,7 +2249,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$W$260</c:f>
+              <c:f>OLD_DATA!$W$260</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2249,7 +2260,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$261:$O$263</c:f>
+              <c:f>OLD_DATA!$O$261:$O$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2267,7 +2278,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$W$261:$W$263</c:f>
+              <c:f>OLD_DATA!$W$261:$W$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2293,11 +2304,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99312768"/>
-        <c:axId val="99314688"/>
+        <c:axId val="123872000"/>
+        <c:axId val="123873920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99312768"/>
+        <c:axId val="123872000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2334,12 +2345,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99314688"/>
+        <c:crossAx val="123873920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99314688"/>
+        <c:axId val="123873920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -2378,7 +2389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99312768"/>
+        <c:crossAx val="123872000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2448,7 +2459,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$293</c:f>
+              <c:f>OLD_DATA!$B$293</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2463,7 +2474,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$294:$W$294</c:f>
+              <c:f>OLD_DATA!$P$294:$W$294</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2496,7 +2507,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$295:$W$295</c:f>
+              <c:f>OLD_DATA!$P$295:$W$295</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2513,11 +2524,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47236992"/>
-        <c:axId val="47931776"/>
+        <c:axId val="123894400"/>
+        <c:axId val="123900672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47236992"/>
+        <c:axId val="123894400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2554,12 +2565,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47931776"/>
+        <c:crossAx val="123900672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47931776"/>
+        <c:axId val="123900672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -2598,7 +2609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47236992"/>
+        <c:crossAx val="123894400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2668,7 +2679,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$297</c:f>
+              <c:f>OLD_DATA!$B$297</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2683,7 +2694,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$298:$Y$298</c:f>
+              <c:f>OLD_DATA!$P$298:$Y$298</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2716,7 +2727,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$299:$Y$299</c:f>
+              <c:f>OLD_DATA!$P$299:$Y$299</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2733,11 +2744,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103072896"/>
-        <c:axId val="108475520"/>
+        <c:axId val="124339328"/>
+        <c:axId val="124341248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103072896"/>
+        <c:axId val="124339328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2774,12 +2785,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="108475520"/>
+        <c:crossAx val="124341248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108475520"/>
+        <c:axId val="124341248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -2818,7 +2829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103072896"/>
+        <c:crossAx val="124339328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3019,11 +3030,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91928064"/>
-        <c:axId val="91929984"/>
+        <c:axId val="119776384"/>
+        <c:axId val="119778304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91928064"/>
+        <c:axId val="119776384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -3048,7 +3059,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3062,12 +3072,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91929984"/>
+        <c:crossAx val="119778304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91929984"/>
+        <c:axId val="119778304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -3099,14 +3109,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91928064"/>
+        <c:crossAx val="119776384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3172,7 +3181,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$29</c:f>
+              <c:f>OLD_DATA!$N$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3187,7 +3196,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$36</c:f>
+              <c:f>OLD_DATA!$B$30:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3217,7 +3226,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$30:$N$36</c:f>
+              <c:f>OLD_DATA!$N$30:$N$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3252,7 +3261,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$29</c:f>
+              <c:f>OLD_DATA!$Q$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3263,7 +3272,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$36</c:f>
+              <c:f>OLD_DATA!$B$30:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3293,7 +3302,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$30:$Q$36</c:f>
+              <c:f>OLD_DATA!$Q$30:$Q$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3331,11 +3340,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92431104"/>
-        <c:axId val="92433024"/>
+        <c:axId val="122179968"/>
+        <c:axId val="122181888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92431104"/>
+        <c:axId val="122179968"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3359,7 +3368,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3373,12 +3381,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92433024"/>
+        <c:crossAx val="122181888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92433024"/>
+        <c:axId val="122181888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -3410,14 +3418,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92431104"/>
+        <c:crossAx val="122179968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3483,7 +3490,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$29</c:f>
+              <c:f>OLD_DATA!$R$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3498,7 +3505,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$36</c:f>
+              <c:f>OLD_DATA!$B$30:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3528,7 +3535,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$30:$R$36</c:f>
+              <c:f>OLD_DATA!$R$30:$R$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3563,7 +3570,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$29</c:f>
+              <c:f>OLD_DATA!$U$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3574,7 +3581,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$36</c:f>
+              <c:f>OLD_DATA!$B$30:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3604,7 +3611,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$U$30:$U$36</c:f>
+              <c:f>OLD_DATA!$U$30:$U$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3642,11 +3649,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92466560"/>
-        <c:axId val="93390336"/>
+        <c:axId val="122213120"/>
+        <c:axId val="122215040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92466560"/>
+        <c:axId val="122213120"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3670,7 +3677,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3684,12 +3690,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93390336"/>
+        <c:crossAx val="122215040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93390336"/>
+        <c:axId val="122215040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -3721,14 +3727,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92466560"/>
+        <c:crossAx val="122213120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3794,7 +3799,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$60</c:f>
+              <c:f>OLD_DATA!$B$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3809,7 +3814,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$61:$Y$61</c:f>
+              <c:f>OLD_DATA!$N$61:$Y$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3854,7 +3859,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$62:$Y$62</c:f>
+              <c:f>OLD_DATA!$N$62:$Y$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3904,7 +3909,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$68</c:f>
+              <c:f>OLD_DATA!$B$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3915,7 +3920,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$69:$Y$69</c:f>
+              <c:f>OLD_DATA!$N$69:$Y$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3960,7 +3965,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$70:$Y$70</c:f>
+              <c:f>OLD_DATA!$N$70:$Y$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4013,11 +4018,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93442048"/>
-        <c:axId val="93443968"/>
+        <c:axId val="122249216"/>
+        <c:axId val="122251136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93442048"/>
+        <c:axId val="122249216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4040,7 +4045,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4054,12 +4058,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93443968"/>
+        <c:crossAx val="122251136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93443968"/>
+        <c:axId val="122251136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -4091,14 +4095,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93442048"/>
+        <c:crossAx val="122249216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4164,7 +4167,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$64</c:f>
+              <c:f>OLD_DATA!$B$64</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4179,7 +4182,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$65:$Y$65</c:f>
+              <c:f>OLD_DATA!$N$65:$Y$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4224,7 +4227,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$66:$Y$66</c:f>
+              <c:f>OLD_DATA!$N$66:$Y$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4274,7 +4277,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$72</c:f>
+              <c:f>OLD_DATA!$B$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4285,7 +4288,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$73:$Y$73</c:f>
+              <c:f>OLD_DATA!$N$73:$Y$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4330,7 +4333,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$74:$Y$74</c:f>
+              <c:f>OLD_DATA!$N$74:$Y$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4383,11 +4386,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96144384"/>
-        <c:axId val="96171136"/>
+        <c:axId val="123222656"/>
+        <c:axId val="123228928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96144384"/>
+        <c:axId val="123222656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4410,7 +4413,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4424,12 +4426,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96171136"/>
+        <c:crossAx val="123228928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96171136"/>
+        <c:axId val="123228928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -4461,14 +4463,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96144384"/>
+        <c:crossAx val="123222656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4534,7 +4535,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$98</c:f>
+              <c:f>OLD_DATA!$B$98</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4549,7 +4550,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$99:$Y$99</c:f>
+              <c:f>OLD_DATA!$N$99:$Y$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4594,7 +4595,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$100:$Y$100</c:f>
+              <c:f>OLD_DATA!$N$100:$Y$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4644,7 +4645,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$106</c:f>
+              <c:f>OLD_DATA!$B$106</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4655,7 +4656,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$107:$Y$107</c:f>
+              <c:f>OLD_DATA!$N$107:$Y$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4700,7 +4701,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$108:$Y$108</c:f>
+              <c:f>OLD_DATA!$N$108:$Y$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4753,11 +4754,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96202752"/>
-        <c:axId val="96204672"/>
+        <c:axId val="123250176"/>
+        <c:axId val="123252096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96202752"/>
+        <c:axId val="123250176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4780,7 +4781,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4794,12 +4794,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96204672"/>
+        <c:crossAx val="123252096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96204672"/>
+        <c:axId val="123252096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -4831,14 +4831,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96202752"/>
+        <c:crossAx val="123250176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4904,7 +4903,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$102</c:f>
+              <c:f>OLD_DATA!$B$102</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4919,7 +4918,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$103:$Y$103</c:f>
+              <c:f>OLD_DATA!$N$103:$Y$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4964,7 +4963,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$104:$Y$104</c:f>
+              <c:f>OLD_DATA!$N$104:$Y$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5014,7 +5013,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$110</c:f>
+              <c:f>OLD_DATA!$B$110</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5025,7 +5024,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$111:$Y$111</c:f>
+              <c:f>OLD_DATA!$N$111:$Y$111</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5070,7 +5069,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$112:$Y$112</c:f>
+              <c:f>OLD_DATA!$N$112:$Y$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5123,11 +5122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96762496"/>
-        <c:axId val="96764672"/>
+        <c:axId val="123263616"/>
+        <c:axId val="123155200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96762496"/>
+        <c:axId val="123263616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5150,7 +5149,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5164,12 +5162,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96764672"/>
+        <c:crossAx val="123155200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96764672"/>
+        <c:axId val="123155200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -5201,14 +5199,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96762496"/>
+        <c:crossAx val="123263616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5274,7 +5271,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$136</c:f>
+              <c:f>OLD_DATA!$N$136</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5289,7 +5286,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$137:$L$140</c:f>
+              <c:f>OLD_DATA!$L$137:$L$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5310,7 +5307,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$137:$N$140</c:f>
+              <c:f>OLD_DATA!$N$137:$N$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5336,7 +5333,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$136</c:f>
+              <c:f>OLD_DATA!$Q$136</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5347,7 +5344,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$137:$L$140</c:f>
+              <c:f>OLD_DATA!$L$137:$L$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5368,7 +5365,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$137:$Q$140</c:f>
+              <c:f>OLD_DATA!$Q$137:$Q$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5397,11 +5394,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96605312"/>
-        <c:axId val="96607232"/>
+        <c:axId val="123204352"/>
+        <c:axId val="123206272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96605312"/>
+        <c:axId val="123204352"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5433,7 +5430,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5447,12 +5443,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96607232"/>
+        <c:crossAx val="123206272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96607232"/>
+        <c:axId val="123206272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -5484,14 +5480,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96605312"/>
+        <c:crossAx val="123204352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5523,6 +5518,252 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>532950</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect b="6772"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5724525" y="76200"/>
+          <a:ext cx="3600000" cy="7591425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47162</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>122966</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9344025" y="104775"/>
+          <a:ext cx="3704762" cy="6876191"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>113855</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85021</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4543425" y="161925"/>
+          <a:ext cx="3561905" cy="5638096"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552035</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>122880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3486150" y="180975"/>
+          <a:ext cx="3323810" cy="7561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>351995</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect b="7661"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7953375" y="171450"/>
+          <a:ext cx="3438095" cy="6877050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390117</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104072</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3990975" y="190500"/>
+          <a:ext cx="3266667" cy="5628572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8151,10 +8392,1406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2460702</v>
+      </c>
+      <c r="C3">
+        <v>120400098</v>
+      </c>
+      <c r="D3">
+        <v>2913515</v>
+      </c>
+      <c r="E3">
+        <v>510352</v>
+      </c>
+      <c r="F3">
+        <v>1950350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2227752</v>
+      </c>
+      <c r="C4">
+        <v>120633048</v>
+      </c>
+      <c r="D4">
+        <v>2913515</v>
+      </c>
+      <c r="E4">
+        <v>548162</v>
+      </c>
+      <c r="F4">
+        <v>1679590</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A41" si="0">A4+1</f>
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2045775</v>
+      </c>
+      <c r="C5">
+        <v>120815025</v>
+      </c>
+      <c r="D5">
+        <v>2913515</v>
+      </c>
+      <c r="E5">
+        <v>640517</v>
+      </c>
+      <c r="F5">
+        <v>1405258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1770367</v>
+      </c>
+      <c r="C6">
+        <v>121090433</v>
+      </c>
+      <c r="D6">
+        <v>2913515</v>
+      </c>
+      <c r="E6">
+        <v>558144</v>
+      </c>
+      <c r="F6">
+        <v>1212223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1573373</v>
+      </c>
+      <c r="C7">
+        <v>121287427</v>
+      </c>
+      <c r="D7">
+        <v>2913515</v>
+      </c>
+      <c r="E7">
+        <v>536458</v>
+      </c>
+      <c r="F7">
+        <v>1036915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>1401572</v>
+      </c>
+      <c r="C8">
+        <v>121459228</v>
+      </c>
+      <c r="D8">
+        <v>2913515</v>
+      </c>
+      <c r="E8">
+        <v>521697</v>
+      </c>
+      <c r="F8">
+        <v>879875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>1243381</v>
+      </c>
+      <c r="C9">
+        <v>121617419</v>
+      </c>
+      <c r="D9">
+        <v>2913515</v>
+      </c>
+      <c r="E9">
+        <v>479163</v>
+      </c>
+      <c r="F9">
+        <v>764218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1101544</v>
+      </c>
+      <c r="C10">
+        <v>121759256</v>
+      </c>
+      <c r="D10">
+        <v>2913515</v>
+      </c>
+      <c r="E10">
+        <v>445078</v>
+      </c>
+      <c r="F10">
+        <v>656466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>975778</v>
+      </c>
+      <c r="C11">
+        <v>121885022</v>
+      </c>
+      <c r="D11">
+        <v>2913515</v>
+      </c>
+      <c r="E11">
+        <v>416082</v>
+      </c>
+      <c r="F11">
+        <v>559696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>839206</v>
+      </c>
+      <c r="C12">
+        <v>122021594</v>
+      </c>
+      <c r="D12">
+        <v>2913515</v>
+      </c>
+      <c r="E12">
+        <v>373529</v>
+      </c>
+      <c r="F12">
+        <v>465677</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>719549</v>
+      </c>
+      <c r="C13">
+        <v>122141251</v>
+      </c>
+      <c r="D13">
+        <v>2913515</v>
+      </c>
+      <c r="E13">
+        <v>342136</v>
+      </c>
+      <c r="F13">
+        <v>377413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>607983</v>
+      </c>
+      <c r="C14">
+        <v>122252817</v>
+      </c>
+      <c r="D14">
+        <v>2913515</v>
+      </c>
+      <c r="E14">
+        <v>315831</v>
+      </c>
+      <c r="F14">
+        <v>292152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>503841</v>
+      </c>
+      <c r="C15">
+        <v>122356959</v>
+      </c>
+      <c r="D15">
+        <v>2913515</v>
+      </c>
+      <c r="E15">
+        <v>282745</v>
+      </c>
+      <c r="F15">
+        <v>221096</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>414436</v>
+      </c>
+      <c r="C16">
+        <v>122446364</v>
+      </c>
+      <c r="D16">
+        <v>2913515</v>
+      </c>
+      <c r="E16">
+        <v>252032</v>
+      </c>
+      <c r="F16">
+        <v>162404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>339370</v>
+      </c>
+      <c r="C17">
+        <v>122521430</v>
+      </c>
+      <c r="D17">
+        <v>2913515</v>
+      </c>
+      <c r="E17">
+        <v>222878</v>
+      </c>
+      <c r="F17">
+        <v>116492</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>278376</v>
+      </c>
+      <c r="C18">
+        <v>122582424</v>
+      </c>
+      <c r="D18">
+        <v>2913515</v>
+      </c>
+      <c r="E18">
+        <v>194702</v>
+      </c>
+      <c r="F18">
+        <v>83674</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>229720</v>
+      </c>
+      <c r="C19">
+        <v>122631080</v>
+      </c>
+      <c r="D19">
+        <v>2913515</v>
+      </c>
+      <c r="E19">
+        <v>168692</v>
+      </c>
+      <c r="F19">
+        <v>61028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>190684</v>
+      </c>
+      <c r="C20">
+        <v>122670116</v>
+      </c>
+      <c r="D20">
+        <v>2913515</v>
+      </c>
+      <c r="E20">
+        <v>144453</v>
+      </c>
+      <c r="F20">
+        <v>46231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>160006</v>
+      </c>
+      <c r="C21">
+        <v>122700794</v>
+      </c>
+      <c r="D21">
+        <v>2913515</v>
+      </c>
+      <c r="E21">
+        <v>123123</v>
+      </c>
+      <c r="F21">
+        <v>36883</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>134997</v>
+      </c>
+      <c r="C22">
+        <v>122725803</v>
+      </c>
+      <c r="D22">
+        <v>2913515</v>
+      </c>
+      <c r="E22">
+        <v>103634</v>
+      </c>
+      <c r="F22">
+        <v>31363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>115746</v>
+      </c>
+      <c r="C23">
+        <v>122745054</v>
+      </c>
+      <c r="D23">
+        <v>2913515</v>
+      </c>
+      <c r="E23">
+        <v>87623</v>
+      </c>
+      <c r="F23">
+        <v>28123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>242337</v>
+      </c>
+      <c r="C3">
+        <v>122618463</v>
+      </c>
+      <c r="D3">
+        <v>2913515</v>
+      </c>
+      <c r="E3">
+        <v>166489</v>
+      </c>
+      <c r="F3">
+        <v>75848</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>131317</v>
+      </c>
+      <c r="C4">
+        <v>122729483</v>
+      </c>
+      <c r="D4">
+        <v>2913515</v>
+      </c>
+      <c r="E4">
+        <v>87604</v>
+      </c>
+      <c r="F4">
+        <v>43713</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>131845</v>
+      </c>
+      <c r="C5">
+        <v>122728955</v>
+      </c>
+      <c r="D5">
+        <v>2913515</v>
+      </c>
+      <c r="E5">
+        <v>102870</v>
+      </c>
+      <c r="F5">
+        <v>28975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>115746</v>
+      </c>
+      <c r="C6">
+        <v>122745054</v>
+      </c>
+      <c r="D6">
+        <v>2913515</v>
+      </c>
+      <c r="E6">
+        <v>87623</v>
+      </c>
+      <c r="F6">
+        <v>28123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>114451</v>
+      </c>
+      <c r="C7">
+        <v>122746349</v>
+      </c>
+      <c r="D7">
+        <v>2913515</v>
+      </c>
+      <c r="E7">
+        <v>91316</v>
+      </c>
+      <c r="F7">
+        <v>23135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>110401</v>
+      </c>
+      <c r="C8">
+        <v>122750399</v>
+      </c>
+      <c r="D8">
+        <v>2913515</v>
+      </c>
+      <c r="E8">
+        <v>86340</v>
+      </c>
+      <c r="F8">
+        <v>24061</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>107615</v>
+      </c>
+      <c r="C9">
+        <v>122753185</v>
+      </c>
+      <c r="D9">
+        <v>2913515</v>
+      </c>
+      <c r="E9">
+        <v>86343</v>
+      </c>
+      <c r="F9">
+        <v>21272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>107465</v>
+      </c>
+      <c r="C10">
+        <v>122753335</v>
+      </c>
+      <c r="D10">
+        <v>2913515</v>
+      </c>
+      <c r="E10">
+        <v>85343</v>
+      </c>
+      <c r="F10">
+        <v>22122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>127729</v>
+      </c>
+      <c r="C3">
+        <v>6342671</v>
+      </c>
+      <c r="D3">
+        <v>152228</v>
+      </c>
+      <c r="E3">
+        <v>27608</v>
+      </c>
+      <c r="F3">
+        <v>100121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>116623</v>
+      </c>
+      <c r="C4">
+        <v>6353777</v>
+      </c>
+      <c r="D4">
+        <v>152228</v>
+      </c>
+      <c r="E4">
+        <v>30115</v>
+      </c>
+      <c r="F4">
+        <v>86508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A23" si="0">A4+1</f>
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>106283</v>
+      </c>
+      <c r="C5">
+        <v>6364117</v>
+      </c>
+      <c r="D5">
+        <v>152228</v>
+      </c>
+      <c r="E5">
+        <v>33817</v>
+      </c>
+      <c r="F5">
+        <v>72466</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>92407</v>
+      </c>
+      <c r="C6">
+        <v>6377993</v>
+      </c>
+      <c r="D6">
+        <v>152228</v>
+      </c>
+      <c r="E6">
+        <v>30425</v>
+      </c>
+      <c r="F6">
+        <v>61982</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>81383</v>
+      </c>
+      <c r="C7">
+        <v>6389017</v>
+      </c>
+      <c r="D7">
+        <v>152228</v>
+      </c>
+      <c r="E7">
+        <v>29169</v>
+      </c>
+      <c r="F7">
+        <v>52214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>71669</v>
+      </c>
+      <c r="C8">
+        <v>6398731</v>
+      </c>
+      <c r="D8">
+        <v>152228</v>
+      </c>
+      <c r="E8">
+        <v>27955</v>
+      </c>
+      <c r="F8">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>64307</v>
+      </c>
+      <c r="C9">
+        <v>6406093</v>
+      </c>
+      <c r="D9">
+        <v>152228</v>
+      </c>
+      <c r="E9">
+        <v>25317</v>
+      </c>
+      <c r="F9">
+        <v>38990</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>57137</v>
+      </c>
+      <c r="C10">
+        <v>6413263</v>
+      </c>
+      <c r="D10">
+        <v>152228</v>
+      </c>
+      <c r="E10">
+        <v>23648</v>
+      </c>
+      <c r="F10">
+        <v>33789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>50200</v>
+      </c>
+      <c r="C11">
+        <v>6420200</v>
+      </c>
+      <c r="D11">
+        <v>152228</v>
+      </c>
+      <c r="E11">
+        <v>21616</v>
+      </c>
+      <c r="F11">
+        <v>28584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>43509</v>
+      </c>
+      <c r="C12">
+        <v>6426891</v>
+      </c>
+      <c r="D12">
+        <v>152228</v>
+      </c>
+      <c r="E12">
+        <v>19434</v>
+      </c>
+      <c r="F12">
+        <v>24075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>37547</v>
+      </c>
+      <c r="C13">
+        <v>6432853</v>
+      </c>
+      <c r="D13">
+        <v>152228</v>
+      </c>
+      <c r="E13">
+        <v>17764</v>
+      </c>
+      <c r="F13">
+        <v>19783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>31949</v>
+      </c>
+      <c r="C14">
+        <v>6438451</v>
+      </c>
+      <c r="D14">
+        <v>152228</v>
+      </c>
+      <c r="E14">
+        <v>16533</v>
+      </c>
+      <c r="F14">
+        <v>15416</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>26675</v>
+      </c>
+      <c r="C15">
+        <v>6443725</v>
+      </c>
+      <c r="D15">
+        <v>152228</v>
+      </c>
+      <c r="E15">
+        <v>14868</v>
+      </c>
+      <c r="F15">
+        <v>11807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>22062</v>
+      </c>
+      <c r="C16">
+        <v>6448338</v>
+      </c>
+      <c r="D16">
+        <v>152228</v>
+      </c>
+      <c r="E16">
+        <v>13371</v>
+      </c>
+      <c r="F16">
+        <v>8691</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>18004</v>
+      </c>
+      <c r="C17">
+        <v>6452396</v>
+      </c>
+      <c r="D17">
+        <v>152228</v>
+      </c>
+      <c r="E17">
+        <v>11764</v>
+      </c>
+      <c r="F17">
+        <v>6240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>14768</v>
+      </c>
+      <c r="C18">
+        <v>6455632</v>
+      </c>
+      <c r="D18">
+        <v>152228</v>
+      </c>
+      <c r="E18">
+        <v>10260</v>
+      </c>
+      <c r="F18">
+        <v>4508</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>12239</v>
+      </c>
+      <c r="C19">
+        <v>6458161</v>
+      </c>
+      <c r="D19">
+        <v>152228</v>
+      </c>
+      <c r="E19">
+        <v>8985</v>
+      </c>
+      <c r="F19">
+        <v>3254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>10154</v>
+      </c>
+      <c r="C20">
+        <v>6460246</v>
+      </c>
+      <c r="D20">
+        <v>152228</v>
+      </c>
+      <c r="E20">
+        <v>7681</v>
+      </c>
+      <c r="F20">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>8689</v>
+      </c>
+      <c r="C21">
+        <v>6461711</v>
+      </c>
+      <c r="D21">
+        <v>152228</v>
+      </c>
+      <c r="E21">
+        <v>6710</v>
+      </c>
+      <c r="F21">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>7420</v>
+      </c>
+      <c r="C22">
+        <v>6462980</v>
+      </c>
+      <c r="D22">
+        <v>152228</v>
+      </c>
+      <c r="E22">
+        <v>5742</v>
+      </c>
+      <c r="F22">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>6322</v>
+      </c>
+      <c r="C23">
+        <v>6464078</v>
+      </c>
+      <c r="D23">
+        <v>152228</v>
+      </c>
+      <c r="E23">
+        <v>4830</v>
+      </c>
+      <c r="F23">
+        <v>1492</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>12868</v>
+      </c>
+      <c r="C3">
+        <v>6457532</v>
+      </c>
+      <c r="D3">
+        <v>152228</v>
+      </c>
+      <c r="E3">
+        <v>8964</v>
+      </c>
+      <c r="F3">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7340</v>
+      </c>
+      <c r="C4">
+        <v>6463060</v>
+      </c>
+      <c r="D4">
+        <v>152228</v>
+      </c>
+      <c r="E4">
+        <v>4772</v>
+      </c>
+      <c r="F4">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>7010</v>
+      </c>
+      <c r="C5">
+        <v>6463390</v>
+      </c>
+      <c r="D5">
+        <v>152228</v>
+      </c>
+      <c r="E5">
+        <v>5544</v>
+      </c>
+      <c r="F5">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6322</v>
+      </c>
+      <c r="C6">
+        <v>6464078</v>
+      </c>
+      <c r="D6">
+        <v>152228</v>
+      </c>
+      <c r="E6">
+        <v>4830</v>
+      </c>
+      <c r="F6">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6168</v>
+      </c>
+      <c r="C7">
+        <v>6464232</v>
+      </c>
+      <c r="D7">
+        <v>152228</v>
+      </c>
+      <c r="E7">
+        <v>4996</v>
+      </c>
+      <c r="F7">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6027</v>
+      </c>
+      <c r="C8">
+        <v>6464373</v>
+      </c>
+      <c r="D8">
+        <v>152228</v>
+      </c>
+      <c r="E8">
+        <v>4823</v>
+      </c>
+      <c r="F8">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>5791</v>
+      </c>
+      <c r="C9">
+        <v>6464609</v>
+      </c>
+      <c r="D9">
+        <v>152228</v>
+      </c>
+      <c r="E9">
+        <v>4761</v>
+      </c>
+      <c r="F9">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>5850</v>
+      </c>
+      <c r="C10">
+        <v>6464550</v>
+      </c>
+      <c r="D10">
+        <v>152228</v>
+      </c>
+      <c r="E10">
+        <v>4807</v>
+      </c>
+      <c r="F10">
+        <v>1043</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B24:AA299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q201" sqref="Q201"/>
+    <sheetView topLeftCell="A275" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P326" sqref="P326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12133,28 +13770,4 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>